<commit_message>
add user story 38 and 39 wrote by Zhe Sun and correct some bugs in the main document to generate the complete output message, add a isWithinXXDays function in class CalculateAge
</commit_message>
<xml_diff>
--- a/Documents/TeamReport.xlsx
+++ b/Documents/TeamReport.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="11013"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="22130"/>
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/michaelwen/Documents/555/homework/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="S:\Courses Info\SSW 555 Agile Dev\lastOne\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E2B32972-7539-5149-B7F5-1BD8901056B2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{92A753F8-B208-4EBA-913C-C1D22C831F4D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="33600" yWindow="2520" windowWidth="30080" windowHeight="33380" tabRatio="500" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" tabRatio="500" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Team" sheetId="1" r:id="rId1"/>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="811" uniqueCount="342">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="869" uniqueCount="382">
   <si>
     <t>Date</t>
     <phoneticPr fontId="2" type="noConversion"/>
@@ -1100,6 +1100,126 @@
   </si>
   <si>
     <t>967-993</t>
+  </si>
+  <si>
+    <t>60mins</t>
+  </si>
+  <si>
+    <t>20mins</t>
+  </si>
+  <si>
+    <t>220mins</t>
+  </si>
+  <si>
+    <t>55mins</t>
+  </si>
+  <si>
+    <t>src/main/java/tools/us31.java</t>
+  </si>
+  <si>
+    <t>src/main/java/tools/us32.java</t>
+  </si>
+  <si>
+    <t>src/main/java/tools/us33.java</t>
+  </si>
+  <si>
+    <t>src/main/java/tools/us34.java</t>
+  </si>
+  <si>
+    <t>src/main/java/tools/us35.java</t>
+  </si>
+  <si>
+    <t>src/main/java/tools/us36.java</t>
+  </si>
+  <si>
+    <t>src/main/java/tools/us37.java</t>
+  </si>
+  <si>
+    <t>src/main/java/tools/us38.java</t>
+  </si>
+  <si>
+    <t>src/main/java/tools/us39.java</t>
+  </si>
+  <si>
+    <t>src/main/java/tools/us42.java</t>
+  </si>
+  <si>
+    <t>us31</t>
+  </si>
+  <si>
+    <t>us32</t>
+  </si>
+  <si>
+    <t>us34</t>
+  </si>
+  <si>
+    <t>us35</t>
+  </si>
+  <si>
+    <t>us36</t>
+  </si>
+  <si>
+    <t>us37</t>
+  </si>
+  <si>
+    <t>us38</t>
+  </si>
+  <si>
+    <t>us39</t>
+  </si>
+  <si>
+    <t>us33</t>
+  </si>
+  <si>
+    <t>us42</t>
+  </si>
+  <si>
+    <t>12-34</t>
+  </si>
+  <si>
+    <t>11-33</t>
+  </si>
+  <si>
+    <t>TestUS31T &amp; F</t>
+  </si>
+  <si>
+    <t>TestUS32T &amp; F</t>
+  </si>
+  <si>
+    <t>TestUS34T &amp; F</t>
+  </si>
+  <si>
+    <t>TestUS35T &amp; F</t>
+  </si>
+  <si>
+    <t>TestUS36T &amp; F</t>
+  </si>
+  <si>
+    <t>TestUS37T &amp; F</t>
+  </si>
+  <si>
+    <t>TestUS38T &amp; F</t>
+  </si>
+  <si>
+    <t>TestUS39T &amp; F</t>
+  </si>
+  <si>
+    <t>TestUS33T &amp; F</t>
+  </si>
+  <si>
+    <t>TestUS42T &amp; F</t>
+  </si>
+  <si>
+    <t>1123-1158</t>
+  </si>
+  <si>
+    <t>1087-1104</t>
+  </si>
+  <si>
+    <t>1048-1083</t>
+  </si>
+  <si>
+    <t>1010-1045</t>
   </si>
 </sst>
 </file>
@@ -1259,7 +1379,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -1304,74 +1424,78 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="66">
-    <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="10" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="14" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="16" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="18" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="20" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="22" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="24" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="26" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="28" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="30" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="32" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="34" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="36" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="38" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="40" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="42" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="44" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="46" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="48" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="50" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="52" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="54" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="56" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="58" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="60" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="62" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="64" builtinId="9" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="9" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="11" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="13" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="15" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="17" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="19" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="21" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="23" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="25" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="27" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="29" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="31" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="33" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="35" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="37" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="39" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="41" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="43" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="45" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="47" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="49" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="51" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="53" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="55" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="57" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="59" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="61" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="63" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="65" builtinId="8"/>
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="已访问的超链接" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="已访问的超链接" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="已访问的超链接" xfId="6" builtinId="9" hidden="1"/>
+    <cellStyle name="已访问的超链接" xfId="8" builtinId="9" hidden="1"/>
+    <cellStyle name="已访问的超链接" xfId="10" builtinId="9" hidden="1"/>
+    <cellStyle name="已访问的超链接" xfId="12" builtinId="9" hidden="1"/>
+    <cellStyle name="已访问的超链接" xfId="14" builtinId="9" hidden="1"/>
+    <cellStyle name="已访问的超链接" xfId="16" builtinId="9" hidden="1"/>
+    <cellStyle name="已访问的超链接" xfId="18" builtinId="9" hidden="1"/>
+    <cellStyle name="已访问的超链接" xfId="20" builtinId="9" hidden="1"/>
+    <cellStyle name="已访问的超链接" xfId="22" builtinId="9" hidden="1"/>
+    <cellStyle name="已访问的超链接" xfId="24" builtinId="9" hidden="1"/>
+    <cellStyle name="已访问的超链接" xfId="26" builtinId="9" hidden="1"/>
+    <cellStyle name="已访问的超链接" xfId="28" builtinId="9" hidden="1"/>
+    <cellStyle name="已访问的超链接" xfId="30" builtinId="9" hidden="1"/>
+    <cellStyle name="已访问的超链接" xfId="32" builtinId="9" hidden="1"/>
+    <cellStyle name="已访问的超链接" xfId="34" builtinId="9" hidden="1"/>
+    <cellStyle name="已访问的超链接" xfId="36" builtinId="9" hidden="1"/>
+    <cellStyle name="已访问的超链接" xfId="38" builtinId="9" hidden="1"/>
+    <cellStyle name="已访问的超链接" xfId="40" builtinId="9" hidden="1"/>
+    <cellStyle name="已访问的超链接" xfId="42" builtinId="9" hidden="1"/>
+    <cellStyle name="已访问的超链接" xfId="44" builtinId="9" hidden="1"/>
+    <cellStyle name="已访问的超链接" xfId="46" builtinId="9" hidden="1"/>
+    <cellStyle name="已访问的超链接" xfId="48" builtinId="9" hidden="1"/>
+    <cellStyle name="已访问的超链接" xfId="50" builtinId="9" hidden="1"/>
+    <cellStyle name="已访问的超链接" xfId="52" builtinId="9" hidden="1"/>
+    <cellStyle name="已访问的超链接" xfId="54" builtinId="9" hidden="1"/>
+    <cellStyle name="已访问的超链接" xfId="56" builtinId="9" hidden="1"/>
+    <cellStyle name="已访问的超链接" xfId="58" builtinId="9" hidden="1"/>
+    <cellStyle name="已访问的超链接" xfId="60" builtinId="9" hidden="1"/>
+    <cellStyle name="已访问的超链接" xfId="62" builtinId="9" hidden="1"/>
+    <cellStyle name="已访问的超链接" xfId="64" builtinId="9" hidden="1"/>
+    <cellStyle name="常规" xfId="0" builtinId="0"/>
+    <cellStyle name="超链接" xfId="1" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="3" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="5" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="7" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="9" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="11" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="13" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="15" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="17" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="19" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="21" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="23" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="25" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="27" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="29" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="31" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="33" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="35" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="37" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="39" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="41" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="43" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="45" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="47" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="49" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="51" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="53" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="55" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="57" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="59" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="61" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="63" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="65" builtinId="8"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
@@ -1389,7 +1513,7 @@
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="1"/>
-  <c:lang val="en-US"/>
+  <c:lang val="zh-CN"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -1413,7 +1537,7 @@
             <c:numRef>
               <c:f>'Burndown README'!$B$15:$B$20</c:f>
               <c:numCache>
-                <c:formatCode>m/d/yy</c:formatCode>
+                <c:formatCode>m/d/yyyy</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
                   <c:v>42263</c:v>
@@ -1484,7 +1608,7 @@
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
-        <c:numFmt formatCode="m/d/yy" sourceLinked="1"/>
+        <c:numFmt formatCode="m/d/yyyy" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -1526,7 +1650,7 @@
 <file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="1"/>
-  <c:lang val="en-US"/>
+  <c:lang val="zh-CN"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -1550,7 +1674,7 @@
             <c:numRef>
               <c:f>Burndown!$A$2:$A$7</c:f>
               <c:numCache>
-                <c:formatCode>m/d/yy</c:formatCode>
+                <c:formatCode>m/d/yyyy</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
                   <c:v>42263</c:v>
@@ -1618,7 +1742,7 @@
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
-        <c:numFmt formatCode="m/d/yy" sourceLinked="1"/>
+        <c:numFmt formatCode="m/d/yyyy" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -2480,9 +2604,9 @@
       <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="13"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.75"/>
   <cols>
-    <col min="1" max="1" width="7.83203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="7.875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="6.5" customWidth="1"/>
     <col min="3" max="3" width="8.5" customWidth="1"/>
     <col min="4" max="4" width="33.5" customWidth="1"/>
@@ -2600,7 +2724,7 @@
       </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:E6">
+  <sortState ref="A2:E6">
     <sortCondition ref="C2"/>
   </sortState>
   <phoneticPr fontId="2" type="noConversion"/>
@@ -2621,17 +2745,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:E41"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" zoomScale="150" workbookViewId="0">
-      <selection activeCell="E32" sqref="E32"/>
+    <sheetView topLeftCell="A22" zoomScale="150" workbookViewId="0">
+      <selection activeCell="C39" sqref="C39"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="13"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.75"/>
   <cols>
     <col min="1" max="1" width="10.5" customWidth="1"/>
-    <col min="2" max="2" width="11.6640625" customWidth="1"/>
-    <col min="3" max="3" width="33.1640625" customWidth="1"/>
-    <col min="4" max="4" width="6.6640625" customWidth="1"/>
-    <col min="5" max="5" width="7.6640625" customWidth="1"/>
+    <col min="2" max="2" width="11.625" customWidth="1"/>
+    <col min="3" max="3" width="33.125" customWidth="1"/>
+    <col min="4" max="4" width="6.625" customWidth="1"/>
+    <col min="5" max="5" width="7.625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" s="4" customFormat="1">
@@ -2651,7 +2775,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="14">
+    <row r="2" spans="1:5">
       <c r="A2">
         <v>1</v>
       </c>
@@ -2668,7 +2792,7 @@
         <v>208</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="14">
+    <row r="3" spans="1:5">
       <c r="A3">
         <v>1</v>
       </c>
@@ -2685,7 +2809,7 @@
         <v>208</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="14">
+    <row r="4" spans="1:5">
       <c r="A4">
         <v>1</v>
       </c>
@@ -2702,7 +2826,7 @@
         <v>208</v>
       </c>
     </row>
-    <row r="5" spans="1:5" ht="14">
+    <row r="5" spans="1:5">
       <c r="A5">
         <v>1</v>
       </c>
@@ -2719,7 +2843,7 @@
         <v>208</v>
       </c>
     </row>
-    <row r="6" spans="1:5" ht="14">
+    <row r="6" spans="1:5">
       <c r="A6">
         <v>1</v>
       </c>
@@ -2736,7 +2860,7 @@
         <v>208</v>
       </c>
     </row>
-    <row r="7" spans="1:5" ht="14">
+    <row r="7" spans="1:5">
       <c r="A7">
         <v>1</v>
       </c>
@@ -2753,7 +2877,7 @@
         <v>208</v>
       </c>
     </row>
-    <row r="8" spans="1:5" ht="14">
+    <row r="8" spans="1:5">
       <c r="A8">
         <v>1</v>
       </c>
@@ -2770,7 +2894,7 @@
         <v>208</v>
       </c>
     </row>
-    <row r="9" spans="1:5" ht="14">
+    <row r="9" spans="1:5">
       <c r="A9">
         <v>1</v>
       </c>
@@ -2787,7 +2911,7 @@
         <v>208</v>
       </c>
     </row>
-    <row r="10" spans="1:5" ht="14">
+    <row r="10" spans="1:5">
       <c r="A10">
         <v>1</v>
       </c>
@@ -2804,7 +2928,7 @@
         <v>208</v>
       </c>
     </row>
-    <row r="11" spans="1:5" ht="14">
+    <row r="11" spans="1:5">
       <c r="A11">
         <v>1</v>
       </c>
@@ -2821,7 +2945,7 @@
         <v>208</v>
       </c>
     </row>
-    <row r="12" spans="1:5" ht="14">
+    <row r="12" spans="1:5">
       <c r="A12">
         <v>2</v>
       </c>
@@ -2838,7 +2962,7 @@
         <v>208</v>
       </c>
     </row>
-    <row r="13" spans="1:5" ht="14">
+    <row r="13" spans="1:5">
       <c r="A13">
         <v>2</v>
       </c>
@@ -2855,7 +2979,7 @@
         <v>208</v>
       </c>
     </row>
-    <row r="14" spans="1:5" ht="14">
+    <row r="14" spans="1:5">
       <c r="A14">
         <v>2</v>
       </c>
@@ -2872,7 +2996,7 @@
         <v>208</v>
       </c>
     </row>
-    <row r="15" spans="1:5" ht="14">
+    <row r="15" spans="1:5">
       <c r="A15">
         <v>2</v>
       </c>
@@ -2889,7 +3013,7 @@
         <v>208</v>
       </c>
     </row>
-    <row r="16" spans="1:5" ht="14">
+    <row r="16" spans="1:5">
       <c r="A16">
         <v>2</v>
       </c>
@@ -2906,7 +3030,7 @@
         <v>208</v>
       </c>
     </row>
-    <row r="17" spans="1:5" ht="14">
+    <row r="17" spans="1:5">
       <c r="A17">
         <v>2</v>
       </c>
@@ -2923,7 +3047,7 @@
         <v>208</v>
       </c>
     </row>
-    <row r="18" spans="1:5" ht="14">
+    <row r="18" spans="1:5">
       <c r="A18">
         <v>2</v>
       </c>
@@ -2940,7 +3064,7 @@
         <v>208</v>
       </c>
     </row>
-    <row r="19" spans="1:5" ht="14">
+    <row r="19" spans="1:5">
       <c r="A19">
         <v>2</v>
       </c>
@@ -2957,7 +3081,7 @@
         <v>208</v>
       </c>
     </row>
-    <row r="20" spans="1:5" ht="14">
+    <row r="20" spans="1:5">
       <c r="A20">
         <v>2</v>
       </c>
@@ -2974,7 +3098,7 @@
         <v>208</v>
       </c>
     </row>
-    <row r="21" spans="1:5" ht="14">
+    <row r="21" spans="1:5">
       <c r="A21">
         <v>2</v>
       </c>
@@ -2991,7 +3115,7 @@
         <v>208</v>
       </c>
     </row>
-    <row r="22" spans="1:5" ht="14">
+    <row r="22" spans="1:5">
       <c r="A22">
         <v>3</v>
       </c>
@@ -3008,7 +3132,7 @@
         <v>208</v>
       </c>
     </row>
-    <row r="23" spans="1:5" ht="14">
+    <row r="23" spans="1:5">
       <c r="A23">
         <v>3</v>
       </c>
@@ -3025,7 +3149,7 @@
         <v>208</v>
       </c>
     </row>
-    <row r="24" spans="1:5" ht="14">
+    <row r="24" spans="1:5">
       <c r="A24">
         <v>3</v>
       </c>
@@ -3042,7 +3166,7 @@
         <v>208</v>
       </c>
     </row>
-    <row r="25" spans="1:5" ht="14">
+    <row r="25" spans="1:5">
       <c r="A25">
         <v>3</v>
       </c>
@@ -3059,7 +3183,7 @@
         <v>208</v>
       </c>
     </row>
-    <row r="26" spans="1:5" ht="14">
+    <row r="26" spans="1:5">
       <c r="A26">
         <v>3</v>
       </c>
@@ -3076,7 +3200,7 @@
         <v>208</v>
       </c>
     </row>
-    <row r="27" spans="1:5" ht="14">
+    <row r="27" spans="1:5">
       <c r="A27">
         <v>3</v>
       </c>
@@ -3093,7 +3217,7 @@
         <v>208</v>
       </c>
     </row>
-    <row r="28" spans="1:5" ht="14">
+    <row r="28" spans="1:5">
       <c r="A28">
         <v>3</v>
       </c>
@@ -3110,7 +3234,7 @@
         <v>208</v>
       </c>
     </row>
-    <row r="29" spans="1:5" ht="14">
+    <row r="29" spans="1:5">
       <c r="A29">
         <v>3</v>
       </c>
@@ -3127,7 +3251,7 @@
         <v>208</v>
       </c>
     </row>
-    <row r="30" spans="1:5" ht="14">
+    <row r="30" spans="1:5">
       <c r="A30">
         <v>3</v>
       </c>
@@ -3144,7 +3268,7 @@
         <v>208</v>
       </c>
     </row>
-    <row r="31" spans="1:5" ht="14">
+    <row r="31" spans="1:5">
       <c r="A31">
         <v>3</v>
       </c>
@@ -3161,7 +3285,7 @@
         <v>208</v>
       </c>
     </row>
-    <row r="32" spans="1:5" ht="14">
+    <row r="32" spans="1:5">
       <c r="A32">
         <v>4</v>
       </c>
@@ -3178,7 +3302,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="33" spans="1:5" ht="14">
+    <row r="33" spans="1:5">
       <c r="A33">
         <v>4</v>
       </c>
@@ -3195,7 +3319,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="34" spans="1:5" ht="14">
+    <row r="34" spans="1:5">
       <c r="A34">
         <v>4</v>
       </c>
@@ -3212,7 +3336,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="35" spans="1:5" ht="14">
+    <row r="35" spans="1:5">
       <c r="A35">
         <v>4</v>
       </c>
@@ -3229,7 +3353,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="36" spans="1:5" ht="14">
+    <row r="36" spans="1:5">
       <c r="A36">
         <v>4</v>
       </c>
@@ -3246,7 +3370,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="37" spans="1:5" ht="14">
+    <row r="37" spans="1:5">
       <c r="A37">
         <v>4</v>
       </c>
@@ -3263,7 +3387,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="38" spans="1:5" ht="14">
+    <row r="38" spans="1:5">
       <c r="A38">
         <v>4</v>
       </c>
@@ -3280,7 +3404,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="39" spans="1:5" ht="14">
+    <row r="39" spans="1:5">
       <c r="A39">
         <v>4</v>
       </c>
@@ -3297,7 +3421,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="40" spans="1:5" ht="14">
+    <row r="40" spans="1:5">
       <c r="A40">
         <v>4</v>
       </c>
@@ -3314,7 +3438,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="41" spans="1:5" ht="14">
+    <row r="41" spans="1:5">
       <c r="A41">
         <v>4</v>
       </c>
@@ -3346,13 +3470,13 @@
       <selection activeCell="F19" sqref="F19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="13"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.75"/>
   <cols>
-    <col min="1" max="1" width="10.83203125" style="7"/>
+    <col min="1" max="1" width="10.875" style="7"/>
     <col min="2" max="2" width="9.5" customWidth="1"/>
-    <col min="3" max="3" width="15.83203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.33203125" customWidth="1"/>
-    <col min="5" max="5" width="6.83203125" customWidth="1"/>
+    <col min="3" max="3" width="15.875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.375" customWidth="1"/>
+    <col min="5" max="5" width="6.875" customWidth="1"/>
     <col min="6" max="6" width="12.5" style="9" customWidth="1"/>
   </cols>
   <sheetData>
@@ -3541,18 +3665,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:F6"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="150" workbookViewId="0">
+    <sheetView zoomScale="150" workbookViewId="0">
       <selection activeCell="F21" sqref="F21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="13"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.75"/>
   <cols>
-    <col min="1" max="1" width="10.83203125" style="2"/>
-    <col min="2" max="2" width="16.6640625" customWidth="1"/>
+    <col min="1" max="1" width="10.875" style="2"/>
+    <col min="2" max="2" width="16.625" customWidth="1"/>
     <col min="3" max="3" width="12.5" customWidth="1"/>
-    <col min="4" max="4" width="7.1640625" customWidth="1"/>
-    <col min="5" max="5" width="6.83203125" customWidth="1"/>
-    <col min="6" max="6" width="20.33203125" style="9" customWidth="1"/>
+    <col min="4" max="4" width="7.125" customWidth="1"/>
+    <col min="5" max="5" width="6.875" customWidth="1"/>
+    <col min="6" max="6" width="20.375" style="9" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" s="4" customFormat="1">
@@ -3681,27 +3805,27 @@
       <selection activeCell="O2" sqref="O2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="13"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.75"/>
   <cols>
-    <col min="1" max="1" width="7.6640625" customWidth="1"/>
+    <col min="1" max="1" width="7.625" customWidth="1"/>
     <col min="2" max="2" width="24.5" style="1" customWidth="1"/>
-    <col min="3" max="3" width="7.33203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.33203125" customWidth="1"/>
-    <col min="5" max="5" width="8.83203125" customWidth="1"/>
-    <col min="6" max="6" width="9.1640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="7.375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.375" customWidth="1"/>
+    <col min="5" max="5" width="8.875" customWidth="1"/>
+    <col min="6" max="6" width="9.125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="8.5" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="9.33203125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="9.375" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="11" style="6" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="37" style="16" customWidth="1"/>
-    <col min="12" max="12" width="19.1640625" style="16" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="19.125" style="16" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="13" style="16" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="1.83203125" style="16" customWidth="1"/>
-    <col min="15" max="15" width="42.33203125" style="16" customWidth="1"/>
-    <col min="16" max="16" width="31.1640625" style="16" customWidth="1"/>
-    <col min="17" max="17" width="10.1640625" style="16" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="1.875" style="16" customWidth="1"/>
+    <col min="15" max="15" width="42.375" style="16" customWidth="1"/>
+    <col min="16" max="16" width="31.125" style="16" customWidth="1"/>
+    <col min="17" max="17" width="10.125" style="16" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" ht="14">
+    <row r="1" spans="1:17">
       <c r="A1" s="4" t="s">
         <v>9</v>
       </c>
@@ -3748,7 +3872,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="2" spans="1:17" ht="14">
+    <row r="2" spans="1:17">
       <c r="A2" t="s">
         <v>112</v>
       </c>
@@ -3797,7 +3921,7 @@
         <v>261</v>
       </c>
     </row>
-    <row r="3" spans="1:17" ht="14">
+    <row r="3" spans="1:17">
       <c r="A3" t="s">
         <v>113</v>
       </c>
@@ -3846,7 +3970,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="4" spans="1:17" ht="14">
+    <row r="4" spans="1:17">
       <c r="A4" t="s">
         <v>114</v>
       </c>
@@ -3895,7 +4019,7 @@
         <v>263</v>
       </c>
     </row>
-    <row r="5" spans="1:17" ht="14">
+    <row r="5" spans="1:17">
       <c r="A5" t="s">
         <v>115</v>
       </c>
@@ -3944,7 +4068,7 @@
         <v>264</v>
       </c>
     </row>
-    <row r="6" spans="1:17" ht="14">
+    <row r="6" spans="1:17">
       <c r="A6" t="s">
         <v>116</v>
       </c>
@@ -3993,7 +4117,7 @@
         <v>265</v>
       </c>
     </row>
-    <row r="7" spans="1:17" ht="14">
+    <row r="7" spans="1:17">
       <c r="A7" t="s">
         <v>117</v>
       </c>
@@ -4042,7 +4166,7 @@
         <v>266</v>
       </c>
     </row>
-    <row r="8" spans="1:17" ht="14">
+    <row r="8" spans="1:17">
       <c r="A8" t="s">
         <v>118</v>
       </c>
@@ -4091,7 +4215,7 @@
         <v>267</v>
       </c>
     </row>
-    <row r="9" spans="1:17" ht="14">
+    <row r="9" spans="1:17">
       <c r="A9" t="s">
         <v>119</v>
       </c>
@@ -4140,7 +4264,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="10" spans="1:17" ht="14">
+    <row r="10" spans="1:17">
       <c r="A10" t="s">
         <v>120</v>
       </c>
@@ -4189,7 +4313,7 @@
         <v>269</v>
       </c>
     </row>
-    <row r="11" spans="1:17" ht="14">
+    <row r="11" spans="1:17">
       <c r="A11" t="s">
         <v>121</v>
       </c>
@@ -4238,18 +4362,18 @@
         <v>270</v>
       </c>
     </row>
-    <row r="14" spans="1:17" ht="14">
+    <row r="14" spans="1:17">
       <c r="B14" s="5" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="15" spans="1:17" ht="14">
+    <row r="15" spans="1:17">
       <c r="B15" s="5" t="s">
         <v>214</v>
       </c>
       <c r="I15" s="7"/>
     </row>
-    <row r="16" spans="1:17" ht="14">
+    <row r="16" spans="1:17">
       <c r="B16" s="5" t="s">
         <v>31</v>
       </c>
@@ -4264,7 +4388,7 @@
       <c r="J16" s="25"/>
       <c r="K16" s="25"/>
     </row>
-    <row r="17" spans="2:11" ht="28">
+    <row r="17" spans="2:11" ht="25.5">
       <c r="B17" s="21" t="s">
         <v>215</v>
       </c>
@@ -4277,7 +4401,7 @@
       <c r="J17" s="25"/>
       <c r="K17" s="25"/>
     </row>
-    <row r="18" spans="2:11" ht="14">
+    <row r="18" spans="2:11">
       <c r="B18" s="21" t="s">
         <v>216</v>
       </c>
@@ -4290,22 +4414,22 @@
       <c r="J18" s="25"/>
       <c r="K18" s="25"/>
     </row>
-    <row r="20" spans="2:11" ht="14">
+    <row r="20" spans="2:11">
       <c r="B20" s="5" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="21" spans="2:11" ht="14">
+    <row r="21" spans="2:11">
       <c r="B21" s="21" t="s">
         <v>217</v>
       </c>
     </row>
-    <row r="22" spans="2:11" ht="14">
+    <row r="22" spans="2:11">
       <c r="B22" s="21" t="s">
         <v>218</v>
       </c>
     </row>
-    <row r="23" spans="2:11" ht="28">
+    <row r="23" spans="2:11" ht="25.5">
       <c r="B23" s="21" t="s">
         <v>219</v>
       </c>
@@ -4328,14 +4452,14 @@
       <selection activeCell="J1" sqref="J1:K11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="13"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.75"/>
   <cols>
-    <col min="2" max="2" width="21.6640625" customWidth="1"/>
-    <col min="11" max="11" width="45.6640625" customWidth="1"/>
-    <col min="15" max="16" width="23.33203125" customWidth="1"/>
+    <col min="2" max="2" width="21.625" customWidth="1"/>
+    <col min="11" max="11" width="45.625" customWidth="1"/>
+    <col min="15" max="16" width="23.375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" ht="14">
+    <row r="1" spans="1:17">
       <c r="A1" s="4" t="s">
         <v>9</v>
       </c>
@@ -4383,7 +4507,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="2" spans="1:17" ht="14">
+    <row r="2" spans="1:17">
       <c r="A2" s="18" t="s">
         <v>122</v>
       </c>
@@ -4430,7 +4554,7 @@
         <v>232</v>
       </c>
     </row>
-    <row r="3" spans="1:17" ht="14">
+    <row r="3" spans="1:17">
       <c r="A3" s="18" t="s">
         <v>123</v>
       </c>
@@ -4477,7 +4601,7 @@
         <v>233</v>
       </c>
     </row>
-    <row r="4" spans="1:17" ht="14">
+    <row r="4" spans="1:17">
       <c r="A4" s="18" t="s">
         <v>124</v>
       </c>
@@ -4524,7 +4648,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="5" spans="1:17" ht="14">
+    <row r="5" spans="1:17">
       <c r="A5" s="18" t="s">
         <v>125</v>
       </c>
@@ -4571,7 +4695,7 @@
         <v>235</v>
       </c>
     </row>
-    <row r="6" spans="1:17" ht="14">
+    <row r="6" spans="1:17">
       <c r="A6" s="18" t="s">
         <v>126</v>
       </c>
@@ -4618,7 +4742,7 @@
         <v>236</v>
       </c>
     </row>
-    <row r="7" spans="1:17" ht="14">
+    <row r="7" spans="1:17">
       <c r="A7" s="18" t="s">
         <v>127</v>
       </c>
@@ -4665,7 +4789,7 @@
         <v>237</v>
       </c>
     </row>
-    <row r="8" spans="1:17" ht="14">
+    <row r="8" spans="1:17">
       <c r="A8" s="18" t="s">
         <v>128</v>
       </c>
@@ -4712,7 +4836,7 @@
         <v>238</v>
       </c>
     </row>
-    <row r="9" spans="1:17" ht="14">
+    <row r="9" spans="1:17">
       <c r="A9" s="18" t="s">
         <v>129</v>
       </c>
@@ -4759,7 +4883,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="10" spans="1:17" ht="14">
+    <row r="10" spans="1:17">
       <c r="A10" s="18" t="s">
         <v>130</v>
       </c>
@@ -4806,7 +4930,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="11" spans="1:17" ht="14">
+    <row r="11" spans="1:17">
       <c r="A11" s="18" t="s">
         <v>131</v>
       </c>
@@ -4863,27 +4987,27 @@
         <v>1050</v>
       </c>
     </row>
-    <row r="14" spans="1:17" ht="14">
+    <row r="14" spans="1:17">
       <c r="B14" s="5" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="15" spans="1:17" ht="14">
+    <row r="15" spans="1:17">
       <c r="B15" s="5" t="s">
         <v>214</v>
       </c>
     </row>
-    <row r="16" spans="1:17" ht="14">
+    <row r="16" spans="1:17">
       <c r="B16" s="5" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="17" spans="2:2" ht="56">
+    <row r="17" spans="2:2" ht="51">
       <c r="B17" s="21" t="s">
         <v>271</v>
       </c>
     </row>
-    <row r="18" spans="2:2" ht="14">
+    <row r="18" spans="2:2">
       <c r="B18" s="21" t="s">
         <v>216</v>
       </c>
@@ -4891,22 +5015,22 @@
     <row r="19" spans="2:2">
       <c r="B19" s="1"/>
     </row>
-    <row r="20" spans="2:2" ht="14">
+    <row r="20" spans="2:2">
       <c r="B20" s="5" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="21" spans="2:2" ht="42">
+    <row r="21" spans="2:2" ht="38.25">
       <c r="B21" s="21" t="s">
         <v>272</v>
       </c>
     </row>
-    <row r="22" spans="2:2" ht="42">
+    <row r="22" spans="2:2" ht="25.5">
       <c r="B22" s="21" t="s">
         <v>274</v>
       </c>
     </row>
-    <row r="23" spans="2:2" ht="28">
+    <row r="23" spans="2:2" ht="25.5">
       <c r="B23" s="21" t="s">
         <v>273</v>
       </c>
@@ -4923,20 +5047,20 @@
   <dimension ref="A1:Q22"/>
   <sheetViews>
     <sheetView zoomScale="150" workbookViewId="0">
-      <selection activeCell="H44" sqref="H44"/>
+      <selection activeCell="M11" sqref="M2:M11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="13"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.75"/>
   <cols>
-    <col min="2" max="2" width="26.83203125" customWidth="1"/>
-    <col min="11" max="11" width="40.33203125" customWidth="1"/>
+    <col min="2" max="2" width="26.875" customWidth="1"/>
+    <col min="11" max="11" width="40.375" customWidth="1"/>
     <col min="13" max="13" width="35.5" customWidth="1"/>
-    <col min="14" max="14" width="23.33203125" customWidth="1"/>
-    <col min="15" max="15" width="27.6640625" customWidth="1"/>
-    <col min="16" max="16" width="31.1640625" customWidth="1"/>
+    <col min="14" max="14" width="23.375" customWidth="1"/>
+    <col min="15" max="15" width="27.625" customWidth="1"/>
+    <col min="16" max="16" width="31.125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" ht="14">
+    <row r="1" spans="1:17">
       <c r="A1" s="4" t="s">
         <v>3</v>
       </c>
@@ -5464,27 +5588,27 @@
         <v>630</v>
       </c>
     </row>
-    <row r="14" spans="1:17" ht="14">
+    <row r="14" spans="1:17">
       <c r="B14" s="5" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="15" spans="1:17" ht="14">
+    <row r="15" spans="1:17">
       <c r="B15" s="21" t="s">
         <v>333</v>
       </c>
     </row>
-    <row r="16" spans="1:17" ht="14">
+    <row r="16" spans="1:17">
       <c r="B16" s="5" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="17" spans="2:2" ht="14">
+    <row r="17" spans="2:2">
       <c r="B17" s="21" t="s">
         <v>335</v>
       </c>
     </row>
-    <row r="18" spans="2:2" ht="56">
+    <row r="18" spans="2:2" ht="51">
       <c r="B18" s="21" t="s">
         <v>334</v>
       </c>
@@ -5492,17 +5616,17 @@
     <row r="19" spans="2:2">
       <c r="B19" s="1"/>
     </row>
-    <row r="20" spans="2:2" ht="14">
+    <row r="20" spans="2:2">
       <c r="B20" s="5" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="21" spans="2:2" ht="28">
+    <row r="21" spans="2:2" ht="25.5">
       <c r="B21" s="1" t="s">
         <v>336</v>
       </c>
     </row>
-    <row r="22" spans="2:2" ht="28">
+    <row r="22" spans="2:2" ht="25.5">
       <c r="B22" s="1" t="s">
         <v>337</v>
       </c>
@@ -5510,20 +5634,32 @@
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
-  <dimension ref="A1:I11"/>
+  <dimension ref="A1:Q11"/>
   <sheetViews>
-    <sheetView zoomScale="150" workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+    <sheetView tabSelected="1" zoomScale="150" workbookViewId="0">
+      <selection activeCell="G15" sqref="G15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="13"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.75"/>
+  <cols>
+    <col min="2" max="2" width="30.75" customWidth="1"/>
+    <col min="3" max="3" width="15.5" customWidth="1"/>
+    <col min="4" max="4" width="6.75" customWidth="1"/>
+    <col min="5" max="5" width="9.25" customWidth="1"/>
+    <col min="6" max="6" width="8.875" style="26" customWidth="1"/>
+    <col min="11" max="11" width="26.625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="15.5" customWidth="1"/>
+    <col min="15" max="15" width="34.25" customWidth="1"/>
+    <col min="16" max="16" width="13.625" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="28">
+    <row r="1" spans="1:17">
       <c r="A1" s="4" t="s">
         <v>3</v>
       </c>
@@ -5551,8 +5687,27 @@
       <c r="I1" s="10" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="2" spans="1:9" ht="14">
+      <c r="K1" s="15" t="s">
+        <v>176</v>
+      </c>
+      <c r="L1" s="15" t="s">
+        <v>178</v>
+      </c>
+      <c r="M1" s="15" t="s">
+        <v>179</v>
+      </c>
+      <c r="N1" s="16"/>
+      <c r="O1" s="15" t="s">
+        <v>177</v>
+      </c>
+      <c r="P1" s="15" t="s">
+        <v>180</v>
+      </c>
+      <c r="Q1" s="15" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="2" spans="1:17">
       <c r="A2" t="s">
         <v>142</v>
       </c>
@@ -5562,14 +5717,28 @@
       <c r="C2" s="20" t="s">
         <v>194</v>
       </c>
-      <c r="D2" s="18" t="s">
-        <v>207</v>
+      <c r="D2" s="20" t="s">
+        <v>208</v>
       </c>
       <c r="E2">
         <v>30</v>
       </c>
-    </row>
-    <row r="3" spans="1:9" ht="14">
+      <c r="K2" s="20" t="s">
+        <v>346</v>
+      </c>
+      <c r="L2" s="20" t="s">
+        <v>356</v>
+      </c>
+      <c r="M2" s="27"/>
+      <c r="O2" s="20" t="s">
+        <v>286</v>
+      </c>
+      <c r="P2" s="20" t="s">
+        <v>368</v>
+      </c>
+      <c r="Q2" s="27"/>
+    </row>
+    <row r="3" spans="1:17">
       <c r="A3" t="s">
         <v>143</v>
       </c>
@@ -5579,14 +5748,28 @@
       <c r="C3" s="20" t="s">
         <v>194</v>
       </c>
-      <c r="D3" s="18" t="s">
-        <v>207</v>
+      <c r="D3" s="20" t="s">
+        <v>208</v>
       </c>
       <c r="E3">
         <v>30</v>
       </c>
-    </row>
-    <row r="4" spans="1:9" ht="14">
+      <c r="K3" s="20" t="s">
+        <v>347</v>
+      </c>
+      <c r="L3" s="20" t="s">
+        <v>357</v>
+      </c>
+      <c r="M3" s="27"/>
+      <c r="O3" s="20" t="s">
+        <v>286</v>
+      </c>
+      <c r="P3" s="20" t="s">
+        <v>369</v>
+      </c>
+      <c r="Q3" s="27"/>
+    </row>
+    <row r="4" spans="1:17">
       <c r="A4" t="s">
         <v>145</v>
       </c>
@@ -5596,14 +5779,28 @@
       <c r="C4" s="20" t="s">
         <v>195</v>
       </c>
-      <c r="D4" s="18" t="s">
-        <v>207</v>
+      <c r="D4" s="20" t="s">
+        <v>208</v>
       </c>
       <c r="E4">
         <v>40</v>
       </c>
-    </row>
-    <row r="5" spans="1:9" ht="14">
+      <c r="K4" s="20" t="s">
+        <v>349</v>
+      </c>
+      <c r="L4" s="20" t="s">
+        <v>358</v>
+      </c>
+      <c r="M4" s="27"/>
+      <c r="O4" s="20" t="s">
+        <v>286</v>
+      </c>
+      <c r="P4" s="20" t="s">
+        <v>370</v>
+      </c>
+      <c r="Q4" s="27"/>
+    </row>
+    <row r="5" spans="1:17">
       <c r="A5" t="s">
         <v>146</v>
       </c>
@@ -5613,14 +5810,28 @@
       <c r="C5" s="20" t="s">
         <v>195</v>
       </c>
-      <c r="D5" s="18" t="s">
-        <v>207</v>
+      <c r="D5" s="20" t="s">
+        <v>208</v>
       </c>
       <c r="E5">
         <v>40</v>
       </c>
-    </row>
-    <row r="6" spans="1:9" ht="14">
+      <c r="K5" s="20" t="s">
+        <v>350</v>
+      </c>
+      <c r="L5" s="20" t="s">
+        <v>359</v>
+      </c>
+      <c r="M5" s="27"/>
+      <c r="O5" s="20" t="s">
+        <v>286</v>
+      </c>
+      <c r="P5" s="20" t="s">
+        <v>371</v>
+      </c>
+      <c r="Q5" s="27"/>
+    </row>
+    <row r="6" spans="1:17">
       <c r="A6" t="s">
         <v>147</v>
       </c>
@@ -5630,14 +5841,30 @@
       <c r="C6" s="20" t="s">
         <v>196</v>
       </c>
-      <c r="D6" s="18" t="s">
-        <v>207</v>
+      <c r="D6" s="20" t="s">
+        <v>208</v>
       </c>
       <c r="E6">
         <v>50</v>
       </c>
-    </row>
-    <row r="7" spans="1:9" ht="14">
+      <c r="K6" s="20" t="s">
+        <v>351</v>
+      </c>
+      <c r="L6" s="20" t="s">
+        <v>360</v>
+      </c>
+      <c r="M6" s="27"/>
+      <c r="O6" s="20" t="s">
+        <v>286</v>
+      </c>
+      <c r="P6" s="20" t="s">
+        <v>372</v>
+      </c>
+      <c r="Q6" s="27" t="s">
+        <v>381</v>
+      </c>
+    </row>
+    <row r="7" spans="1:17">
       <c r="A7" t="s">
         <v>148</v>
       </c>
@@ -5647,14 +5874,30 @@
       <c r="C7" s="20" t="s">
         <v>196</v>
       </c>
-      <c r="D7" s="18" t="s">
-        <v>207</v>
+      <c r="D7" s="20" t="s">
+        <v>208</v>
       </c>
       <c r="E7">
         <v>50</v>
       </c>
-    </row>
-    <row r="8" spans="1:9" ht="14">
+      <c r="K7" s="20" t="s">
+        <v>352</v>
+      </c>
+      <c r="L7" s="20" t="s">
+        <v>361</v>
+      </c>
+      <c r="M7" s="27"/>
+      <c r="O7" s="20" t="s">
+        <v>286</v>
+      </c>
+      <c r="P7" s="20" t="s">
+        <v>373</v>
+      </c>
+      <c r="Q7" s="27" t="s">
+        <v>380</v>
+      </c>
+    </row>
+    <row r="8" spans="1:17">
       <c r="A8" t="s">
         <v>149</v>
       </c>
@@ -5664,14 +5907,44 @@
       <c r="C8" s="20" t="s">
         <v>193</v>
       </c>
-      <c r="D8" s="18" t="s">
-        <v>207</v>
+      <c r="D8" s="20" t="s">
+        <v>208</v>
       </c>
       <c r="E8">
         <v>40</v>
       </c>
-    </row>
-    <row r="9" spans="1:9" ht="14">
+      <c r="F8" s="26" t="s">
+        <v>342</v>
+      </c>
+      <c r="G8">
+        <v>71</v>
+      </c>
+      <c r="H8" t="s">
+        <v>344</v>
+      </c>
+      <c r="I8" t="s">
+        <v>211</v>
+      </c>
+      <c r="K8" s="20" t="s">
+        <v>353</v>
+      </c>
+      <c r="L8" s="20" t="s">
+        <v>362</v>
+      </c>
+      <c r="M8" s="27" t="s">
+        <v>367</v>
+      </c>
+      <c r="O8" s="20" t="s">
+        <v>286</v>
+      </c>
+      <c r="P8" s="20" t="s">
+        <v>374</v>
+      </c>
+      <c r="Q8" s="27" t="s">
+        <v>379</v>
+      </c>
+    </row>
+    <row r="9" spans="1:17">
       <c r="A9" t="s">
         <v>150</v>
       </c>
@@ -5681,14 +5954,44 @@
       <c r="C9" s="20" t="s">
         <v>193</v>
       </c>
-      <c r="D9" s="18" t="s">
-        <v>207</v>
+      <c r="D9" s="20" t="s">
+        <v>208</v>
       </c>
       <c r="E9">
         <v>40</v>
       </c>
-    </row>
-    <row r="10" spans="1:9" ht="14">
+      <c r="F9" s="26" t="s">
+        <v>343</v>
+      </c>
+      <c r="G9">
+        <v>22</v>
+      </c>
+      <c r="H9" t="s">
+        <v>345</v>
+      </c>
+      <c r="I9" t="s">
+        <v>211</v>
+      </c>
+      <c r="K9" s="20" t="s">
+        <v>354</v>
+      </c>
+      <c r="L9" s="20" t="s">
+        <v>363</v>
+      </c>
+      <c r="M9" s="27" t="s">
+        <v>366</v>
+      </c>
+      <c r="O9" s="20" t="s">
+        <v>286</v>
+      </c>
+      <c r="P9" s="20" t="s">
+        <v>375</v>
+      </c>
+      <c r="Q9" s="27" t="s">
+        <v>378</v>
+      </c>
+    </row>
+    <row r="10" spans="1:17">
       <c r="A10" t="s">
         <v>144</v>
       </c>
@@ -5698,14 +6001,28 @@
       <c r="C10" s="20" t="s">
         <v>209</v>
       </c>
-      <c r="D10" s="18" t="s">
-        <v>207</v>
+      <c r="D10" s="20" t="s">
+        <v>208</v>
       </c>
       <c r="E10">
         <v>20</v>
       </c>
-    </row>
-    <row r="11" spans="1:9" ht="14">
+      <c r="K10" s="20" t="s">
+        <v>348</v>
+      </c>
+      <c r="L10" s="20" t="s">
+        <v>364</v>
+      </c>
+      <c r="M10" s="27"/>
+      <c r="O10" s="20" t="s">
+        <v>286</v>
+      </c>
+      <c r="P10" s="20" t="s">
+        <v>376</v>
+      </c>
+      <c r="Q10" s="27"/>
+    </row>
+    <row r="11" spans="1:17">
       <c r="A11" t="s">
         <v>153</v>
       </c>
@@ -5715,16 +6032,31 @@
       <c r="C11" s="20" t="s">
         <v>209</v>
       </c>
-      <c r="D11" s="18" t="s">
-        <v>207</v>
+      <c r="D11" s="20" t="s">
+        <v>208</v>
       </c>
       <c r="E11">
         <v>40</v>
       </c>
+      <c r="K11" s="20" t="s">
+        <v>355</v>
+      </c>
+      <c r="L11" s="20" t="s">
+        <v>365</v>
+      </c>
+      <c r="M11" s="27"/>
+      <c r="O11" s="20" t="s">
+        <v>286</v>
+      </c>
+      <c r="P11" s="20" t="s">
+        <v>377</v>
+      </c>
+      <c r="Q11" s="27"/>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -5732,17 +6064,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
   <dimension ref="A1:C43"/>
   <sheetViews>
-    <sheetView topLeftCell="A27" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection activeCell="A34" sqref="A34:B34"/>
+    <sheetView topLeftCell="A25" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="13"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.75"/>
   <cols>
-    <col min="2" max="2" width="28.1640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="28.125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="49.5" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" s="4" customFormat="1" ht="14">
+    <row r="1" spans="1:3" s="4" customFormat="1">
       <c r="A1" s="4" t="s">
         <v>111</v>
       </c>
@@ -5753,7 +6085,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="34">
+    <row r="2" spans="1:3" ht="31.5">
       <c r="A2" t="s">
         <v>112</v>
       </c>
@@ -5764,7 +6096,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="3" spans="1:3" ht="17">
+    <row r="3" spans="1:3" ht="15.75">
       <c r="A3" t="s">
         <v>113</v>
       </c>
@@ -5775,7 +6107,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="17">
+    <row r="4" spans="1:3" ht="15.75">
       <c r="A4" t="s">
         <v>114</v>
       </c>
@@ -5786,7 +6118,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="5" spans="1:3" ht="34">
+    <row r="5" spans="1:3" ht="31.5">
       <c r="A5" t="s">
         <v>115</v>
       </c>
@@ -5797,7 +6129,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="6" spans="1:3" ht="17">
+    <row r="6" spans="1:3" ht="15.75">
       <c r="A6" t="s">
         <v>116</v>
       </c>
@@ -5808,7 +6140,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="7" spans="1:3" ht="17">
+    <row r="7" spans="1:3" ht="15.75">
       <c r="A7" t="s">
         <v>117</v>
       </c>
@@ -5819,7 +6151,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="8" spans="1:3" ht="51">
+    <row r="8" spans="1:3" ht="47.25">
       <c r="A8" t="s">
         <v>118</v>
       </c>
@@ -5830,7 +6162,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="9" spans="1:3" ht="34">
+    <row r="9" spans="1:3" ht="31.5">
       <c r="A9" t="s">
         <v>119</v>
       </c>
@@ -5841,7 +6173,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="10" spans="1:3" ht="34">
+    <row r="10" spans="1:3" ht="31.5">
       <c r="A10" t="s">
         <v>120</v>
       </c>
@@ -5852,7 +6184,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="11" spans="1:3" ht="34">
+    <row r="11" spans="1:3" ht="31.5">
       <c r="A11" t="s">
         <v>121</v>
       </c>
@@ -5863,7 +6195,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="12" spans="1:3" ht="34">
+    <row r="12" spans="1:3" ht="31.5">
       <c r="A12" t="s">
         <v>122</v>
       </c>
@@ -5874,7 +6206,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="13" spans="1:3" ht="51">
+    <row r="13" spans="1:3" ht="47.25">
       <c r="A13" t="s">
         <v>123</v>
       </c>
@@ -5885,7 +6217,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="14" spans="1:3" ht="68">
+    <row r="14" spans="1:3" ht="63">
       <c r="A14" t="s">
         <v>124</v>
       </c>
@@ -5896,7 +6228,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="15" spans="1:3" ht="34">
+    <row r="15" spans="1:3" ht="31.5">
       <c r="A15" t="s">
         <v>125</v>
       </c>
@@ -5907,7 +6239,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="16" spans="1:3" ht="17">
+    <row r="16" spans="1:3" ht="15.75">
       <c r="A16" t="s">
         <v>126</v>
       </c>
@@ -5918,7 +6250,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="17" spans="1:3" ht="34">
+    <row r="17" spans="1:3" ht="31.5">
       <c r="A17" t="s">
         <v>127</v>
       </c>
@@ -5929,7 +6261,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="18" spans="1:3" ht="17">
+    <row r="18" spans="1:3" ht="15.75">
       <c r="A18" t="s">
         <v>128</v>
       </c>
@@ -5940,7 +6272,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="19" spans="1:3" ht="17">
+    <row r="19" spans="1:3" ht="15.75">
       <c r="A19" t="s">
         <v>129</v>
       </c>
@@ -5951,7 +6283,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="20" spans="1:3" ht="17">
+    <row r="20" spans="1:3" ht="15.75">
       <c r="A20" t="s">
         <v>130</v>
       </c>
@@ -5962,7 +6294,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="21" spans="1:3" ht="34">
+    <row r="21" spans="1:3" ht="31.5">
       <c r="A21" t="s">
         <v>131</v>
       </c>
@@ -5973,7 +6305,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="22" spans="1:3" ht="34">
+    <row r="22" spans="1:3" ht="31.5">
       <c r="A22" t="s">
         <v>132</v>
       </c>
@@ -5984,7 +6316,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="23" spans="1:3" ht="34">
+    <row r="23" spans="1:3" ht="31.5">
       <c r="A23" t="s">
         <v>133</v>
       </c>
@@ -5995,7 +6327,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="24" spans="1:3" ht="34">
+    <row r="24" spans="1:3" ht="31.5">
       <c r="A24" t="s">
         <v>134</v>
       </c>
@@ -6006,7 +6338,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="25" spans="1:3" ht="51">
+    <row r="25" spans="1:3" ht="47.25">
       <c r="A25" t="s">
         <v>135</v>
       </c>
@@ -6017,7 +6349,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="26" spans="1:3" ht="34">
+    <row r="26" spans="1:3" ht="31.5">
       <c r="A26" t="s">
         <v>136</v>
       </c>
@@ -6028,7 +6360,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="27" spans="1:3" ht="136">
+    <row r="27" spans="1:3" ht="126">
       <c r="A27" t="s">
         <v>137</v>
       </c>
@@ -6039,7 +6371,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="28" spans="1:3" ht="17">
+    <row r="28" spans="1:3" ht="15.75">
       <c r="A28" t="s">
         <v>138</v>
       </c>
@@ -6050,7 +6382,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="29" spans="1:3" ht="34">
+    <row r="29" spans="1:3" ht="31.5">
       <c r="A29" t="s">
         <v>139</v>
       </c>
@@ -6061,7 +6393,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="30" spans="1:3" ht="17">
+    <row r="30" spans="1:3" ht="15.75">
       <c r="A30" t="s">
         <v>140</v>
       </c>
@@ -6072,7 +6404,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="31" spans="1:3" ht="17">
+    <row r="31" spans="1:3" ht="15.75">
       <c r="A31" t="s">
         <v>141</v>
       </c>
@@ -6083,7 +6415,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="32" spans="1:3" ht="34">
+    <row r="32" spans="1:3" ht="31.5">
       <c r="A32" t="s">
         <v>142</v>
       </c>
@@ -6094,7 +6426,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="33" spans="1:3" ht="17">
+    <row r="33" spans="1:3" ht="15.75">
       <c r="A33" t="s">
         <v>143</v>
       </c>
@@ -6105,7 +6437,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="34" spans="1:3" ht="34">
+    <row r="34" spans="1:3" ht="31.5">
       <c r="A34" t="s">
         <v>144</v>
       </c>
@@ -6116,7 +6448,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="35" spans="1:3" ht="51">
+    <row r="35" spans="1:3" ht="47.25">
       <c r="A35" t="s">
         <v>145</v>
       </c>
@@ -6127,7 +6459,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="36" spans="1:3" ht="34">
+    <row r="36" spans="1:3" ht="31.5">
       <c r="A36" t="s">
         <v>146</v>
       </c>
@@ -6138,7 +6470,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="37" spans="1:3" ht="34">
+    <row r="37" spans="1:3" ht="31.5">
       <c r="A37" t="s">
         <v>147</v>
       </c>
@@ -6149,7 +6481,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="38" spans="1:3" ht="34">
+    <row r="38" spans="1:3" ht="31.5">
       <c r="A38" t="s">
         <v>148</v>
       </c>
@@ -6160,7 +6492,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="39" spans="1:3" ht="34">
+    <row r="39" spans="1:3" ht="31.5">
       <c r="A39" t="s">
         <v>149</v>
       </c>
@@ -6171,7 +6503,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="40" spans="1:3" ht="34">
+    <row r="40" spans="1:3" ht="31.5">
       <c r="A40" t="s">
         <v>150</v>
       </c>
@@ -6182,7 +6514,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="41" spans="1:3" ht="34">
+    <row r="41" spans="1:3" ht="31.5">
       <c r="A41" t="s">
         <v>151</v>
       </c>
@@ -6193,7 +6525,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="42" spans="1:3" ht="34">
+    <row r="42" spans="1:3" ht="31.5">
       <c r="A42" t="s">
         <v>152</v>
       </c>
@@ -6204,7 +6536,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="43" spans="1:3" ht="34">
+    <row r="43" spans="1:3" ht="31.5">
       <c r="A43" t="s">
         <v>153</v>
       </c>

</xml_diff>